<commit_message>
fix time_type database files
</commit_message>
<xml_diff>
--- a/database/industries/chemical/shamla/balancesheet/quarterly.xlsx
+++ b/database/industries/chemical/shamla/balancesheet/quarterly.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="e:\Trade\database\industries\chemical\shamla\balancesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB5560D4-795E-449C-835D-0C73BABB2219}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7350"/>
+    <workbookView xWindow="2640" yWindow="1704" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="65">
   <si>
     <t>Pouya Finance</t>
   </si>
@@ -36,37 +37,37 @@
     <t>دوره مالی</t>
   </si>
   <si>
-    <t>فصل چهارم منتهی به 1396/12</t>
-  </si>
-  <si>
-    <t>فصل چهارم منتهی به 1397/12</t>
-  </si>
-  <si>
-    <t>فصل چهارم منتهی به 1398/12</t>
-  </si>
-  <si>
-    <t>فصل چهارم منتهی به 1399/12</t>
+    <t>فصل دوم منتهی به 1400/06</t>
+  </si>
+  <si>
+    <t>فصل سوم منتهی به 1400/09</t>
   </si>
   <si>
     <t>فصل چهارم منتهی به 1400/12</t>
   </si>
   <si>
+    <t>فصل اول منتهی به 1401/03</t>
+  </si>
+  <si>
+    <t>فصل دوم منتهی به 1401/06</t>
+  </si>
+  <si>
     <t>تاریخ انتشار</t>
   </si>
   <si>
-    <t>1398-02-04 (9)</t>
-  </si>
-  <si>
-    <t>1399-02-13 (8)</t>
-  </si>
-  <si>
-    <t>1400-02-11 (8)</t>
-  </si>
-  <si>
-    <t>1401-02-22 (10)</t>
+    <t>1400-08-24 (2)</t>
+  </si>
+  <si>
+    <t>1400-10-30</t>
   </si>
   <si>
     <t>1401-08-30 (5)</t>
+  </si>
+  <si>
+    <t>1401-04-29</t>
+  </si>
+  <si>
+    <t>1401-08-30 (2)</t>
   </si>
   <si>
     <t>دارایی</t>
@@ -219,7 +220,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -417,7 +418,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -429,7 +430,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -476,6 +477,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -511,6 +529,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -662,19 +697,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:H59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="67" customWidth="1"/>
     <col min="3" max="3" width="5" customWidth="1"/>
-    <col min="4" max="8" width="31" customWidth="1"/>
+    <col min="4" max="5" width="29" customWidth="1"/>
+    <col min="6" max="6" width="31" customWidth="1"/>
+    <col min="7" max="8" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -683,7 +720,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -694,7 +731,7 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
@@ -705,7 +742,7 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -714,7 +751,7 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="2:8" ht="42" x14ac:dyDescent="0.65">
+    <row r="5" spans="2:8" ht="40.799999999999997" x14ac:dyDescent="0.75">
       <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
@@ -725,7 +762,7 @@
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
     </row>
-    <row r="6" spans="2:8" ht="42" x14ac:dyDescent="0.65">
+    <row r="6" spans="2:8" ht="40.799999999999997" x14ac:dyDescent="0.75">
       <c r="B6" s="5" t="s">
         <v>3</v>
       </c>
@@ -736,7 +773,7 @@
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -745,7 +782,7 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B8" s="7" t="s">
         <v>4</v>
       </c>
@@ -766,7 +803,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B9" s="8" t="s">
         <v>10</v>
       </c>
@@ -787,7 +824,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B10" s="10"/>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
@@ -796,7 +833,7 @@
       <c r="G10" s="11"/>
       <c r="H10" s="11"/>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B11" s="12" t="s">
         <v>16</v>
       </c>
@@ -807,205 +844,205 @@
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B12" s="14" t="s">
         <v>17</v>
       </c>
       <c r="C12" s="15"/>
       <c r="D12" s="15">
-        <v>165230</v>
+        <v>494905</v>
       </c>
       <c r="E12" s="15">
-        <v>301192</v>
+        <v>343805</v>
       </c>
       <c r="F12" s="15">
-        <v>472253</v>
+        <v>408558</v>
       </c>
       <c r="G12" s="15">
-        <v>209224</v>
+        <v>561404</v>
       </c>
       <c r="H12" s="15">
-        <v>408558</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+        <v>964465</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B13" s="10" t="s">
         <v>18</v>
       </c>
       <c r="C13" s="11"/>
       <c r="D13" s="11">
-        <v>73529</v>
+        <v>445978</v>
       </c>
       <c r="E13" s="11">
-        <v>544542</v>
+        <v>263568</v>
       </c>
       <c r="F13" s="11">
-        <v>973752</v>
+        <v>724259</v>
       </c>
       <c r="G13" s="11">
-        <v>357539</v>
+        <v>752697</v>
       </c>
       <c r="H13" s="11">
-        <v>724259</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+        <v>772394</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B14" s="14" t="s">
         <v>19</v>
       </c>
       <c r="C14" s="15"/>
       <c r="D14" s="15">
-        <v>72865</v>
+        <v>494764</v>
       </c>
       <c r="E14" s="15">
-        <v>82349</v>
+        <v>523142</v>
       </c>
       <c r="F14" s="15">
-        <v>299900</v>
+        <v>745413</v>
       </c>
       <c r="G14" s="15">
-        <v>232383</v>
+        <v>743227</v>
       </c>
       <c r="H14" s="15">
-        <v>745413</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+        <v>540184</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B15" s="10" t="s">
         <v>20</v>
       </c>
       <c r="C15" s="11"/>
       <c r="D15" s="11">
-        <v>178022</v>
+        <v>1300874</v>
       </c>
       <c r="E15" s="11">
-        <v>283593</v>
+        <v>1405006</v>
       </c>
       <c r="F15" s="11">
-        <v>340283</v>
+        <v>1746826</v>
       </c>
       <c r="G15" s="11">
-        <v>814258</v>
+        <v>1920616</v>
       </c>
       <c r="H15" s="11">
-        <v>1746826</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+        <v>2165535</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B16" s="14" t="s">
         <v>21</v>
       </c>
       <c r="C16" s="15"/>
       <c r="D16" s="15">
-        <v>3695</v>
+        <v>181976</v>
       </c>
       <c r="E16" s="15">
-        <v>50134</v>
+        <v>142979</v>
       </c>
       <c r="F16" s="15">
-        <v>16860</v>
+        <v>128992</v>
       </c>
       <c r="G16" s="15">
-        <v>212362</v>
+        <v>101484</v>
       </c>
       <c r="H16" s="15">
-        <v>128992</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+        <v>45820</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B17" s="10" t="s">
         <v>22</v>
       </c>
       <c r="C17" s="11"/>
       <c r="D17" s="11">
-        <v>0</v>
+        <v>54959</v>
       </c>
       <c r="E17" s="11">
-        <v>0</v>
+        <v>54959</v>
       </c>
       <c r="F17" s="11">
-        <v>54959</v>
+        <v>0</v>
       </c>
       <c r="G17" s="11">
-        <v>54959</v>
+        <v>0</v>
       </c>
       <c r="H17" s="11">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B18" s="16" t="s">
         <v>23</v>
       </c>
       <c r="C18" s="17"/>
       <c r="D18" s="17">
-        <v>493341</v>
+        <v>2973456</v>
       </c>
       <c r="E18" s="17">
-        <v>1261810</v>
+        <v>2733459</v>
       </c>
       <c r="F18" s="17">
-        <v>2158007</v>
+        <v>3754048</v>
       </c>
       <c r="G18" s="17">
-        <v>1880725</v>
+        <v>4079428</v>
       </c>
       <c r="H18" s="17">
-        <v>3754048</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+        <v>4488398</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B19" s="10" t="s">
         <v>24</v>
       </c>
       <c r="C19" s="11"/>
       <c r="D19" s="11">
-        <v>1711</v>
+        <v>10112</v>
       </c>
       <c r="E19" s="11">
-        <v>2032</v>
+        <v>5604</v>
       </c>
       <c r="F19" s="11">
-        <v>5088</v>
+        <v>5597</v>
       </c>
       <c r="G19" s="11">
-        <v>7958</v>
+        <v>8626</v>
       </c>
       <c r="H19" s="11">
-        <v>5597</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+        <v>8353</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B20" s="14" t="s">
         <v>25</v>
       </c>
       <c r="C20" s="15"/>
       <c r="D20" s="15">
-        <v>145523</v>
+        <v>422095</v>
       </c>
       <c r="E20" s="15">
-        <v>147867</v>
+        <v>625419</v>
       </c>
       <c r="F20" s="15">
-        <v>188622</v>
+        <v>485582</v>
       </c>
       <c r="G20" s="15">
-        <v>425780</v>
+        <v>485679</v>
       </c>
       <c r="H20" s="15">
-        <v>485582</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+        <v>571682</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B21" s="10" t="s">
         <v>26</v>
       </c>
       <c r="C21" s="11"/>
       <c r="D21" s="11">
-        <v>54911</v>
+        <v>0</v>
       </c>
       <c r="E21" s="11">
-        <v>54959</v>
+        <v>0</v>
       </c>
       <c r="F21" s="11">
         <v>0</v>
@@ -1017,49 +1054,49 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B22" s="14" t="s">
         <v>27</v>
       </c>
       <c r="C22" s="15"/>
       <c r="D22" s="15">
-        <v>360620</v>
+        <v>4476583</v>
       </c>
       <c r="E22" s="15">
-        <v>455752</v>
+        <v>4926734</v>
       </c>
       <c r="F22" s="15">
-        <v>917658</v>
+        <v>5287107</v>
       </c>
       <c r="G22" s="15">
-        <v>3216747</v>
+        <v>5808039</v>
       </c>
       <c r="H22" s="15">
-        <v>5287107</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+        <v>6180503</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B23" s="10" t="s">
         <v>28</v>
       </c>
       <c r="C23" s="11"/>
       <c r="D23" s="11">
-        <v>63131</v>
+        <v>41345</v>
       </c>
       <c r="E23" s="11">
-        <v>93106</v>
+        <v>39185</v>
       </c>
       <c r="F23" s="11">
-        <v>43716</v>
+        <v>44189</v>
       </c>
       <c r="G23" s="11">
-        <v>41502</v>
+        <v>40319</v>
       </c>
       <c r="H23" s="11">
-        <v>44189</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+        <v>41803</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B24" s="14" t="s">
         <v>29</v>
       </c>
@@ -1080,70 +1117,70 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B25" s="10" t="s">
         <v>31</v>
       </c>
       <c r="C25" s="11"/>
       <c r="D25" s="11">
-        <v>2130</v>
+        <v>103859</v>
       </c>
       <c r="E25" s="11">
-        <v>2349</v>
+        <v>96578</v>
       </c>
       <c r="F25" s="11">
-        <v>13461</v>
+        <v>247313</v>
       </c>
       <c r="G25" s="11">
-        <v>285364</v>
+        <v>268717</v>
       </c>
       <c r="H25" s="11">
-        <v>247313</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+        <v>161959</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B26" s="16" t="s">
         <v>32</v>
       </c>
       <c r="C26" s="17"/>
       <c r="D26" s="17">
-        <v>628026</v>
+        <v>5053994</v>
       </c>
       <c r="E26" s="17">
-        <v>756065</v>
+        <v>5693520</v>
       </c>
       <c r="F26" s="17">
-        <v>1168545</v>
+        <v>6069788</v>
       </c>
       <c r="G26" s="17">
-        <v>3977351</v>
+        <v>6611380</v>
       </c>
       <c r="H26" s="17">
-        <v>6069788</v>
-      </c>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+        <v>6964300</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B27" s="18" t="s">
         <v>33</v>
       </c>
       <c r="C27" s="19"/>
       <c r="D27" s="19">
-        <v>1121367</v>
+        <v>8027450</v>
       </c>
       <c r="E27" s="19">
-        <v>2017875</v>
+        <v>8426979</v>
       </c>
       <c r="F27" s="19">
-        <v>3326552</v>
+        <v>9823836</v>
       </c>
       <c r="G27" s="19">
-        <v>5858076</v>
+        <v>10690808</v>
       </c>
       <c r="H27" s="19">
-        <v>9823836</v>
-      </c>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+        <v>11452698</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B28" s="12" t="s">
         <v>34</v>
       </c>
@@ -1154,28 +1191,28 @@
       <c r="G28" s="13"/>
       <c r="H28" s="13"/>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B29" s="14" t="s">
         <v>35</v>
       </c>
       <c r="C29" s="15"/>
       <c r="D29" s="15">
-        <v>49868</v>
+        <v>824599</v>
       </c>
       <c r="E29" s="15">
-        <v>104605</v>
+        <v>612278</v>
       </c>
       <c r="F29" s="15">
-        <v>378611</v>
+        <v>944569</v>
       </c>
       <c r="G29" s="15">
-        <v>722691</v>
+        <v>1035446</v>
       </c>
       <c r="H29" s="15">
-        <v>944569</v>
-      </c>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+        <v>1565482</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B30" s="10" t="s">
         <v>36</v>
       </c>
@@ -1196,97 +1233,97 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B31" s="14" t="s">
         <v>37</v>
       </c>
       <c r="C31" s="15"/>
       <c r="D31" s="15">
-        <v>7639</v>
+        <v>0</v>
       </c>
       <c r="E31" s="15">
-        <v>71992</v>
+        <v>186095</v>
       </c>
       <c r="F31" s="15">
-        <v>38240</v>
+        <v>59615</v>
       </c>
       <c r="G31" s="15">
-        <v>188728</v>
+        <v>112236</v>
       </c>
       <c r="H31" s="15">
-        <v>59615</v>
-      </c>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+        <v>75819</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B32" s="10" t="s">
         <v>38</v>
       </c>
       <c r="C32" s="11"/>
       <c r="D32" s="11">
-        <v>126375</v>
+        <v>239887</v>
       </c>
       <c r="E32" s="11">
-        <v>196596</v>
+        <v>312591</v>
       </c>
       <c r="F32" s="11">
-        <v>133943</v>
+        <v>461730</v>
       </c>
       <c r="G32" s="11">
-        <v>463320</v>
+        <v>557950</v>
       </c>
       <c r="H32" s="11">
-        <v>461730</v>
-      </c>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+        <v>263754</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B33" s="14" t="s">
         <v>39</v>
       </c>
       <c r="C33" s="15"/>
       <c r="D33" s="15">
-        <v>0</v>
+        <v>2072165</v>
       </c>
       <c r="E33" s="15">
-        <v>0</v>
+        <v>260243</v>
       </c>
       <c r="F33" s="15">
         <v>0</v>
       </c>
       <c r="G33" s="15">
-        <v>0</v>
+        <v>2822400</v>
       </c>
       <c r="H33" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+        <v>2221331</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B34" s="10" t="s">
         <v>40</v>
       </c>
       <c r="C34" s="11"/>
       <c r="D34" s="11">
-        <v>100716</v>
+        <v>1237806</v>
       </c>
       <c r="E34" s="11">
-        <v>200358</v>
+        <v>998218</v>
       </c>
       <c r="F34" s="11">
-        <v>386789</v>
+        <v>876669</v>
       </c>
       <c r="G34" s="11">
-        <v>886905</v>
+        <v>573906</v>
       </c>
       <c r="H34" s="11">
-        <v>876669</v>
-      </c>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+        <v>766499</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B35" s="14" t="s">
         <v>41</v>
       </c>
       <c r="C35" s="15"/>
       <c r="D35" s="15">
-        <v>0</v>
+        <v>190285</v>
       </c>
       <c r="E35" s="15">
         <v>0</v>
@@ -1301,7 +1338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B36" s="10" t="s">
         <v>42</v>
       </c>
@@ -1322,28 +1359,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B37" s="16" t="s">
         <v>43</v>
       </c>
       <c r="C37" s="17"/>
       <c r="D37" s="17">
-        <v>284598</v>
+        <v>4564742</v>
       </c>
       <c r="E37" s="17">
-        <v>573551</v>
+        <v>2369425</v>
       </c>
       <c r="F37" s="17">
-        <v>937583</v>
+        <v>2342583</v>
       </c>
       <c r="G37" s="17">
-        <v>2261644</v>
+        <v>5101938</v>
       </c>
       <c r="H37" s="17">
-        <v>2342583</v>
-      </c>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+        <v>4892885</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B38" s="10" t="s">
         <v>44</v>
       </c>
@@ -1364,13 +1401,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B39" s="14" t="s">
         <v>45</v>
       </c>
       <c r="C39" s="15"/>
-      <c r="D39" s="15">
-        <v>0</v>
+      <c r="D39" s="15" t="s">
+        <v>30</v>
       </c>
       <c r="E39" s="15" t="s">
         <v>30</v>
@@ -1385,91 +1422,91 @@
         <v>30</v>
       </c>
     </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B40" s="10" t="s">
         <v>46</v>
       </c>
       <c r="C40" s="11"/>
       <c r="D40" s="11">
-        <v>0</v>
+        <v>804355</v>
       </c>
       <c r="E40" s="11">
-        <v>0</v>
+        <v>836899</v>
       </c>
       <c r="F40" s="11">
-        <v>0</v>
+        <v>882269</v>
       </c>
       <c r="G40" s="11">
-        <v>186036</v>
+        <v>916487</v>
       </c>
       <c r="H40" s="11">
-        <v>882269</v>
-      </c>
-    </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+        <v>906745</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B41" s="14" t="s">
         <v>47</v>
       </c>
       <c r="C41" s="15"/>
       <c r="D41" s="15">
-        <v>72492</v>
+        <v>154090</v>
       </c>
       <c r="E41" s="15">
-        <v>67754</v>
+        <v>137603</v>
       </c>
       <c r="F41" s="15">
-        <v>72098</v>
+        <v>170032</v>
       </c>
       <c r="G41" s="15">
-        <v>106124</v>
+        <v>265158</v>
       </c>
       <c r="H41" s="15">
-        <v>170032</v>
-      </c>
-    </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+        <v>272908</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B42" s="18" t="s">
         <v>48</v>
       </c>
       <c r="C42" s="19"/>
       <c r="D42" s="19">
-        <v>72492</v>
+        <v>958445</v>
       </c>
       <c r="E42" s="19">
-        <v>67754</v>
+        <v>974502</v>
       </c>
       <c r="F42" s="19">
-        <v>72098</v>
+        <v>1052301</v>
       </c>
       <c r="G42" s="19">
-        <v>292160</v>
+        <v>1181645</v>
       </c>
       <c r="H42" s="19">
-        <v>1052301</v>
-      </c>
-    </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+        <v>1179653</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B43" s="16" t="s">
         <v>49</v>
       </c>
       <c r="C43" s="17"/>
       <c r="D43" s="17">
-        <v>357090</v>
+        <v>5523187</v>
       </c>
       <c r="E43" s="17">
-        <v>641305</v>
+        <v>3343927</v>
       </c>
       <c r="F43" s="17">
-        <v>1009681</v>
+        <v>3394884</v>
       </c>
       <c r="G43" s="17">
-        <v>2553804</v>
+        <v>6283583</v>
       </c>
       <c r="H43" s="17">
-        <v>3394884</v>
-      </c>
-    </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+        <v>6072538</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B44" s="12" t="s">
         <v>50</v>
       </c>
@@ -1480,28 +1517,28 @@
       <c r="G44" s="13"/>
       <c r="H44" s="13"/>
     </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B45" s="14" t="s">
         <v>51</v>
       </c>
       <c r="C45" s="15"/>
       <c r="D45" s="15">
-        <v>210000</v>
+        <v>840000</v>
       </c>
       <c r="E45" s="15">
-        <v>210000</v>
+        <v>840000</v>
       </c>
       <c r="F45" s="15">
-        <v>210000</v>
+        <v>840000</v>
       </c>
       <c r="G45" s="15">
-        <v>420000</v>
+        <v>840000</v>
       </c>
       <c r="H45" s="15">
-        <v>840000</v>
-      </c>
-    </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+        <v>2700000</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B46" s="10" t="s">
         <v>52</v>
       </c>
@@ -1522,7 +1559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B47" s="14" t="s">
         <v>53</v>
       </c>
@@ -1531,46 +1568,46 @@
         <v>0</v>
       </c>
       <c r="E47" s="15">
-        <v>0</v>
+        <v>1603501</v>
       </c>
       <c r="F47" s="15">
-        <v>210000</v>
+        <v>1799360</v>
       </c>
       <c r="G47" s="15">
-        <v>420000</v>
+        <v>1799419</v>
       </c>
       <c r="H47" s="15">
-        <v>1799360</v>
-      </c>
-    </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B48" s="10" t="s">
         <v>54</v>
       </c>
       <c r="C48" s="11"/>
       <c r="D48" s="11">
-        <v>0</v>
+        <v>-203324</v>
       </c>
       <c r="E48" s="11">
         <v>0</v>
       </c>
       <c r="F48" s="11">
-        <v>0</v>
+        <v>-203324</v>
       </c>
       <c r="G48" s="11">
-        <v>-153644</v>
+        <v>-203324</v>
       </c>
       <c r="H48" s="11">
-        <v>-203324</v>
-      </c>
-    </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
+        <v>-203320</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B49" s="14" t="s">
         <v>55</v>
       </c>
       <c r="C49" s="15"/>
-      <c r="D49" s="15" t="s">
-        <v>30</v>
+      <c r="D49" s="15">
+        <v>0</v>
       </c>
       <c r="E49" s="15">
         <v>0</v>
@@ -1585,28 +1622,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B50" s="10" t="s">
         <v>56</v>
       </c>
       <c r="C50" s="11"/>
       <c r="D50" s="11">
-        <v>21000</v>
+        <v>84000</v>
       </c>
       <c r="E50" s="11">
-        <v>21000</v>
+        <v>84000</v>
       </c>
       <c r="F50" s="11">
-        <v>21000</v>
+        <v>84000</v>
       </c>
       <c r="G50" s="11">
-        <v>42000</v>
+        <v>84000</v>
       </c>
       <c r="H50" s="11">
-        <v>84000</v>
-      </c>
-    </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+        <v>169648</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B51" s="14" t="s">
         <v>57</v>
       </c>
@@ -1627,13 +1664,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B52" s="10" t="s">
         <v>58</v>
       </c>
       <c r="C52" s="11"/>
-      <c r="D52" s="11">
-        <v>0</v>
+      <c r="D52" s="11" t="s">
+        <v>30</v>
       </c>
       <c r="E52" s="11" t="s">
         <v>30</v>
@@ -1648,7 +1685,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B53" s="14" t="s">
         <v>59</v>
       </c>
@@ -1669,13 +1706,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B54" s="10" t="s">
         <v>60</v>
       </c>
       <c r="C54" s="11"/>
-      <c r="D54" s="11">
-        <v>0</v>
+      <c r="D54" s="11" t="s">
+        <v>30</v>
       </c>
       <c r="E54" s="11" t="s">
         <v>30</v>
@@ -1690,7 +1727,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B55" s="14" t="s">
         <v>61</v>
       </c>
@@ -1711,70 +1748,70 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B56" s="10" t="s">
         <v>62</v>
       </c>
       <c r="C56" s="11"/>
       <c r="D56" s="11">
-        <v>533277</v>
+        <v>1783587</v>
       </c>
       <c r="E56" s="11">
-        <v>1145570</v>
+        <v>2555551</v>
       </c>
       <c r="F56" s="11">
-        <v>1875871</v>
+        <v>3908916</v>
       </c>
       <c r="G56" s="11">
-        <v>2575916</v>
+        <v>1887130</v>
       </c>
       <c r="H56" s="11">
-        <v>3908916</v>
-      </c>
-    </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
+        <v>2713832</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B57" s="16" t="s">
         <v>63</v>
       </c>
       <c r="C57" s="17"/>
       <c r="D57" s="17">
-        <v>764277</v>
+        <v>2504263</v>
       </c>
       <c r="E57" s="17">
-        <v>1376570</v>
+        <v>5083052</v>
       </c>
       <c r="F57" s="17">
-        <v>2316871</v>
+        <v>6428952</v>
       </c>
       <c r="G57" s="17">
-        <v>3304272</v>
+        <v>4407225</v>
       </c>
       <c r="H57" s="17">
-        <v>6428952</v>
-      </c>
-    </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
+        <v>5380160</v>
+      </c>
+    </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B58" s="18" t="s">
         <v>64</v>
       </c>
       <c r="C58" s="19"/>
       <c r="D58" s="19">
-        <v>1121367</v>
+        <v>8027450</v>
       </c>
       <c r="E58" s="19">
-        <v>2017875</v>
+        <v>8426979</v>
       </c>
       <c r="F58" s="19">
-        <v>3326552</v>
+        <v>9823836</v>
       </c>
       <c r="G58" s="19">
-        <v>5858076</v>
+        <v>10690808</v>
       </c>
       <c r="H58" s="19">
-        <v>9823836</v>
-      </c>
-    </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
+        <v>11452698</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>

</xml_diff>